<commit_message>
Increased effectiveness of equity portfolio, need to increase covered call strategy now
</commit_message>
<xml_diff>
--- a/portfolio_risk_metrics.xlsx
+++ b/portfolio_risk_metrics.xlsx
@@ -468,67 +468,67 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Equity Portfolio (70%)</t>
+          <t>Equity Portfolio</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>112.582027116127</v>
+        <v>127.137217321074</v>
       </c>
       <c r="C2" t="n">
-        <v>13.49789341778731</v>
+        <v>14.76687513140331</v>
       </c>
       <c r="D2" t="n">
-        <v>19.86807428786387</v>
+        <v>24.05919947431317</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5787120206617425</v>
+        <v>0.5306442196895986</v>
       </c>
       <c r="F2" t="n">
-        <v>-34.45692066436602</v>
+        <v>-34.39828036199673</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Covered Call Strategy (30%)</t>
+          <t>Covered Call Strategy</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>105.1974695313859</v>
+        <v>104.4209511983805</v>
       </c>
       <c r="C3" t="n">
-        <v>12.82619866656123</v>
+        <v>12.75440364326808</v>
       </c>
       <c r="D3" t="n">
-        <v>18.96778008027154</v>
+        <v>17.92061497814814</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5707678294847798</v>
+        <v>0.6001135371962217</v>
       </c>
       <c r="F3" t="n">
-        <v>-34.05311107310756</v>
+        <v>-30.60266810485754</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Combined Portfolio (70/30)</t>
+          <t>Combined Portfolio</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>111.0894103536849</v>
+        <v>123.5200755309552</v>
       </c>
       <c r="C4" t="n">
-        <v>13.36370911358418</v>
+        <v>14.45798093377535</v>
       </c>
       <c r="D4" t="n">
-        <v>19.2840289876177</v>
+        <v>21.18622196611397</v>
       </c>
       <c r="E4" t="n">
-        <v>0.589280856240199</v>
+        <v>0.5880227703505186</v>
       </c>
       <c r="F4" t="n">
-        <v>-34.33485441527328</v>
+        <v>-33.1950418168004</v>
       </c>
     </row>
     <row r="5">
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>125.1811487001833</v>
+        <v>125.1812014728365</v>
       </c>
       <c r="C5" t="n">
-        <v>14.60034466669096</v>
+        <v>14.6003491757158</v>
       </c>
       <c r="D5" t="n">
-        <v>19.70242487607504</v>
+        <v>19.70244352451648</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6395326842226285</v>
+        <v>0.6395323077585131</v>
       </c>
       <c r="F5" t="n">
-        <v>-33.71725745991026</v>
+        <v>-33.71726063766723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Beating the S&P but still higher vol
</commit_message>
<xml_diff>
--- a/portfolio_risk_metrics.xlsx
+++ b/portfolio_risk_metrics.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>127.137217321074</v>
+        <v>127.1380827900173</v>
       </c>
       <c r="C2" t="n">
-        <v>14.76687513140331</v>
+        <v>14.76694854878704</v>
       </c>
       <c r="D2" t="n">
-        <v>24.05919947431317</v>
+        <v>24.05914751908062</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5306442196895986</v>
+        <v>0.5306484171420429</v>
       </c>
       <c r="F2" t="n">
-        <v>-34.39828036199673</v>
+        <v>-34.39788897619459</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>104.4209511983805</v>
+        <v>115.5339339835694</v>
       </c>
       <c r="C3" t="n">
-        <v>12.75440364326808</v>
+        <v>13.76097388637143</v>
       </c>
       <c r="D3" t="n">
-        <v>17.92061497814814</v>
+        <v>21.96153982216473</v>
       </c>
       <c r="E3" t="n">
-        <v>0.6001135371962217</v>
+        <v>0.535525923118635</v>
       </c>
       <c r="F3" t="n">
-        <v>-30.60266810485754</v>
+        <v>-32.89429586848028</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>123.5200755309552</v>
+        <v>127.7648191289491</v>
       </c>
       <c r="C4" t="n">
-        <v>14.45798093377535</v>
+        <v>14.82005332479621</v>
       </c>
       <c r="D4" t="n">
-        <v>21.18622196611397</v>
+        <v>22.08230085818211</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5880227703505186</v>
+        <v>0.5805578597597099</v>
       </c>
       <c r="F4" t="n">
-        <v>-33.1950418168004</v>
+        <v>-33.798272187123</v>
       </c>
     </row>
     <row r="5">
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>125.1812014728365</v>
+        <v>125.1811487001833</v>
       </c>
       <c r="C5" t="n">
-        <v>14.6003491757158</v>
+        <v>14.60034466669096</v>
       </c>
       <c r="D5" t="n">
-        <v>19.70244352451648</v>
+        <v>19.7024414893409</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6395323077585131</v>
+        <v>0.639532144963242</v>
       </c>
       <c r="F5" t="n">
-        <v>-33.71726063766723</v>
+        <v>-33.71726721796418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhanced covered calls and a lot more stable of a portfolio now with increased returns compared to SPY
</commit_message>
<xml_diff>
--- a/portfolio_risk_metrics.xlsx
+++ b/portfolio_risk_metrics.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>127.1380827900173</v>
+        <v>127.1376995041531</v>
       </c>
       <c r="C2" t="n">
-        <v>14.76694854878704</v>
+        <v>14.76691603482945</v>
       </c>
       <c r="D2" t="n">
-        <v>24.05914751908062</v>
+        <v>24.05913949500928</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5306484171420429</v>
+        <v>0.5306472427028307</v>
       </c>
       <c r="F2" t="n">
-        <v>-34.39788897619459</v>
+        <v>-34.39790091985317</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>115.5339339835694</v>
+        <v>182.3086931523248</v>
       </c>
       <c r="C3" t="n">
-        <v>13.76097388637143</v>
+        <v>19.03405453747926</v>
       </c>
       <c r="D3" t="n">
-        <v>21.96153982216473</v>
+        <v>19.38685065985675</v>
       </c>
       <c r="E3" t="n">
-        <v>0.535525923118635</v>
+        <v>0.8786395911508574</v>
       </c>
       <c r="F3" t="n">
-        <v>-32.89429586848028</v>
+        <v>-15.18092499036337</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>127.7648191289491</v>
+        <v>151.5557324430735</v>
       </c>
       <c r="C4" t="n">
-        <v>14.82005332479621</v>
+        <v>16.75129530213459</v>
       </c>
       <c r="D4" t="n">
-        <v>22.08230085818211</v>
+        <v>19.87258352320957</v>
       </c>
       <c r="E4" t="n">
-        <v>0.5805578597597099</v>
+        <v>0.7422937880676802</v>
       </c>
       <c r="F4" t="n">
-        <v>-33.798272187123</v>
+        <v>-24.98145958204303</v>
       </c>
     </row>
     <row r="5">
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>125.1811487001833</v>
+        <v>125.1811750865068</v>
       </c>
       <c r="C5" t="n">
-        <v>14.60034466669096</v>
+        <v>14.60034692120322</v>
       </c>
       <c r="D5" t="n">
-        <v>19.7024414893409</v>
+        <v>19.70244516213175</v>
       </c>
       <c r="E5" t="n">
-        <v>0.639532144963242</v>
+        <v>0.6395321401742148</v>
       </c>
       <c r="F5" t="n">
-        <v>-33.71726721796418</v>
+        <v>-33.71725745991026</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This looks really solid now
</commit_message>
<xml_diff>
--- a/portfolio_risk_metrics.xlsx
+++ b/portfolio_risk_metrics.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>127.1376995041531</v>
+        <v>116.5487521575342</v>
       </c>
       <c r="C2" t="n">
-        <v>14.76691603482945</v>
+        <v>14.64110773955345</v>
       </c>
       <c r="D2" t="n">
-        <v>24.05913949500928</v>
+        <v>24.7105577116583</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5306472427028307</v>
+        <v>0.5115670753796644</v>
       </c>
       <c r="F2" t="n">
-        <v>-34.39790091985317</v>
+        <v>-32.61347595620919</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>182.3086931523248</v>
+        <v>162.8709063428561</v>
       </c>
       <c r="C3" t="n">
-        <v>19.03405453747926</v>
+        <v>18.63918410888486</v>
       </c>
       <c r="D3" t="n">
-        <v>19.38685065985675</v>
+        <v>18.08007757919806</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8786395911508574</v>
+        <v>0.9203049066575347</v>
       </c>
       <c r="F3" t="n">
-        <v>-15.18092499036337</v>
+        <v>-20.60966163179796</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>151.5557324430735</v>
+        <v>134.0590482873069</v>
       </c>
       <c r="C4" t="n">
-        <v>16.75129530213459</v>
+        <v>16.22840751237609</v>
       </c>
       <c r="D4" t="n">
-        <v>19.87258352320957</v>
+        <v>21.35107836877604</v>
       </c>
       <c r="E4" t="n">
-        <v>0.7422937880676802</v>
+        <v>0.6664022896934239</v>
       </c>
       <c r="F4" t="n">
-        <v>-24.98145958204303</v>
+        <v>-28.97331600649987</v>
       </c>
     </row>
     <row r="5">
@@ -538,19 +538,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>125.1811750865068</v>
+        <v>113.6633471380184</v>
       </c>
       <c r="C5" t="n">
-        <v>14.60034692120322</v>
+        <v>14.36948150595614</v>
       </c>
       <c r="D5" t="n">
-        <v>19.70244516213175</v>
+        <v>20.06771767036929</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6395321401742148</v>
+        <v>0.616387060508636</v>
       </c>
       <c r="F5" t="n">
-        <v>-33.71725745991026</v>
+        <v>-33.71726392781539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Enhanced visuals for inspecting the porrtfolio further
</commit_message>
<xml_diff>
--- a/portfolio_risk_metrics.xlsx
+++ b/portfolio_risk_metrics.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>116.5487521575342</v>
+        <v>116.5489338610195</v>
       </c>
       <c r="C2" t="n">
-        <v>14.64110773955345</v>
+        <v>14.64112475069557</v>
       </c>
       <c r="D2" t="n">
-        <v>24.7105577116583</v>
+        <v>24.7105669314315</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5115670753796644</v>
+        <v>0.5115675729242875</v>
       </c>
       <c r="F2" t="n">
-        <v>-32.61347595620919</v>
+        <v>-32.61347782271692</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>162.8709063428561</v>
+        <v>162.8710208505783</v>
       </c>
       <c r="C3" t="n">
-        <v>18.63918410888486</v>
+        <v>18.63919324803902</v>
       </c>
       <c r="D3" t="n">
-        <v>18.08007757919806</v>
+        <v>18.08006915612256</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9203049066575347</v>
+        <v>0.9203058408880254</v>
       </c>
       <c r="F3" t="n">
-        <v>-20.60966163179796</v>
+        <v>-20.60966734199285</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>134.0590482873069</v>
+        <v>134.0592181397132</v>
       </c>
       <c r="C4" t="n">
-        <v>16.22840751237609</v>
+        <v>16.22842242809202</v>
       </c>
       <c r="D4" t="n">
-        <v>21.35107836877604</v>
+        <v>21.35108308835045</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6664022896934239</v>
+        <v>0.6664028409807139</v>
       </c>
       <c r="F4" t="n">
-        <v>-28.97331600649987</v>
+        <v>-28.97332006058485</v>
       </c>
     </row>
     <row r="5">
@@ -538,16 +538,16 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>113.6633471380184</v>
+        <v>113.6633946501941</v>
       </c>
       <c r="C5" t="n">
-        <v>14.36948150595614</v>
+        <v>14.36948600345105</v>
       </c>
       <c r="D5" t="n">
-        <v>20.06771767036929</v>
+        <v>20.0677154066075</v>
       </c>
       <c r="E5" t="n">
-        <v>0.616387060508636</v>
+        <v>0.6163873541568299</v>
       </c>
       <c r="F5" t="n">
         <v>-33.71726392781539</v>

</xml_diff>

<commit_message>
Save location of visuals updated
</commit_message>
<xml_diff>
--- a/portfolio_risk_metrics.xlsx
+++ b/portfolio_risk_metrics.xlsx
@@ -472,19 +472,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>116.5489338610195</v>
+        <v>116.5490096074609</v>
       </c>
       <c r="C2" t="n">
-        <v>14.64112475069557</v>
+        <v>14.6411318420997</v>
       </c>
       <c r="D2" t="n">
-        <v>24.7105669314315</v>
+        <v>24.71057925957926</v>
       </c>
       <c r="E2" t="n">
-        <v>0.5115675729242875</v>
+        <v>0.5115676046808679</v>
       </c>
       <c r="F2" t="n">
-        <v>-32.61347782271692</v>
+        <v>-32.6134954716561</v>
       </c>
     </row>
     <row r="3">
@@ -494,19 +494,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>162.8710208505783</v>
+        <v>162.871030214647</v>
       </c>
       <c r="C3" t="n">
-        <v>18.63919324803902</v>
+        <v>18.63919399540914</v>
       </c>
       <c r="D3" t="n">
-        <v>18.08006915612256</v>
+        <v>18.08007012742409</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9203058408880254</v>
+        <v>0.920305832783834</v>
       </c>
       <c r="F3" t="n">
-        <v>-20.60966734199285</v>
+        <v>-20.60967482631652</v>
       </c>
     </row>
     <row r="4">
@@ -516,19 +516,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>134.0592181397132</v>
+        <v>134.0592763181961</v>
       </c>
       <c r="C4" t="n">
-        <v>16.22842242809202</v>
+        <v>16.2284275370769</v>
       </c>
       <c r="D4" t="n">
-        <v>21.35108308835045</v>
+        <v>21.35109392942267</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6664028409807139</v>
+        <v>0.6664027418974326</v>
       </c>
       <c r="F4" t="n">
-        <v>-28.97332006058485</v>
+        <v>-28.97333324614369</v>
       </c>
     </row>
     <row r="5">
@@ -544,13 +544,13 @@
         <v>14.36948600345105</v>
       </c>
       <c r="D5" t="n">
-        <v>20.0677154066075</v>
+        <v>20.06771397130849</v>
       </c>
       <c r="E5" t="n">
-        <v>0.6163873541568299</v>
+        <v>0.6163873982425768</v>
       </c>
       <c r="F5" t="n">
-        <v>-33.71726392781539</v>
+        <v>-33.71726233893722</v>
       </c>
     </row>
   </sheetData>

</xml_diff>